<commit_message>
DEV-11590 - Added importing of responsibilities to examples and refactored the input-file-examples module to run tests with all the example files provided in the resources folder without having the need to choose and configure what test needs to be run.
</commit_message>
<xml_diff>
--- a/input-file-examples/src/test/resources/add-community-domain-assets-with-responsibilities/responsibilities.xlsx
+++ b/input-file-examples/src/test/resources/add-community-domain-assets-with-responsibilities/responsibilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piotrlandzwojczak/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vidhya.sitaraman@collibra.com/projects/import-api-examples/input-file-examples/src/test/resources/add-community-domain-assets-with-responsibilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC2A87BE-0491-F64E-AF9E-19981D731AD6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077C27F4-2141-DD47-98E9-3B789D267D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39800" yWindow="9120" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relations" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Type</t>
   </si>
@@ -69,28 +69,16 @@
     <t>DB_COLUMN</t>
   </si>
   <si>
-    <t>Roles &gt; Data Steward &gt; User Name</t>
-  </si>
-  <si>
-    <t>Roles &gt; Data Steward &gt; Group Id</t>
-  </si>
-  <si>
-    <t>Roles &gt; Data Steward &gt; Group Name</t>
-  </si>
-  <si>
-    <t>Roles &gt; Reviewer &gt; User Id</t>
-  </si>
-  <si>
-    <t>john.doe</t>
-  </si>
-  <si>
-    <t>471f5852-1d19-4d74-a70f-989100c3c878</t>
-  </si>
-  <si>
-    <t>Data Citizens</t>
-  </si>
-  <si>
-    <t>e060bb6e-df51-466f-903f-af08142c2e9a</t>
+    <t>00000000-0000-0000-0000-000001000003</t>
+  </si>
+  <si>
+    <t>00000000-0000-0000-0000-000000900003</t>
+  </si>
+  <si>
+    <t>Roles &gt; Group Id</t>
+  </si>
+  <si>
+    <t>Roles &gt; User Id</t>
   </si>
 </sst>
 </file>
@@ -512,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -525,14 +513,12 @@
     <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -549,19 +535,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -577,14 +557,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -600,11 +577,11 @@
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -619,9 +596,6 @@
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>